<commit_message>
Addition of additional empty columns to TnT heatmap and cleanup of code
</commit_message>
<xml_diff>
--- a/Analysis Temp X vs X/Secondary Analyses/CF39 25_vs_OtherTemps/TnT CF39 thermoregulation Shrunk2.xlsx
+++ b/Analysis Temp X vs X/Secondary Analyses/CF39 25_vs_OtherTemps/TnT CF39 thermoregulation Shrunk2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Dropbox\Harrison Lab - DATA\TdcA\RNASeq CF39_S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Dropbox\Harrison Lab - Trevor Randall\RNASeq Analysis\RNASeqAnlyPkrat_2020_03\Analysis Temp X vs X\Secondary Analyses\CF39 25_vs_OtherTemps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="65">
   <si>
     <t>PROKKA_06325_sense</t>
   </si>
@@ -41,9 +41,6 @@
     <t>PROKKA_06328_antis</t>
   </si>
   <si>
-    <t>wspR_8</t>
-  </si>
-  <si>
     <t>PROKKA_06333_sense</t>
   </si>
   <si>
@@ -126,6 +123,102 @@
   </si>
   <si>
     <t>PA0459 like protein</t>
+  </si>
+  <si>
+    <t>PROKKA_06326_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06327_sense</t>
+  </si>
+  <si>
+    <t>htpX_2</t>
+  </si>
+  <si>
+    <t>heat shock protein htpX</t>
+  </si>
+  <si>
+    <t>putative membrane protein</t>
+  </si>
+  <si>
+    <t>PROKKA_06329_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06330_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06331_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06332_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06335_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06336_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06337_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06341_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06343_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06344_sense</t>
+  </si>
+  <si>
+    <t>kefB_4</t>
+  </si>
+  <si>
+    <t>wspR_8 (TdcA)</t>
+  </si>
+  <si>
+    <t>glutathione-regulated potassium-efflux system protein KefB</t>
+  </si>
+  <si>
+    <t>trxA_4</t>
+  </si>
+  <si>
+    <t>thioredoxin</t>
+  </si>
+  <si>
+    <t>ftsH_3</t>
+  </si>
+  <si>
+    <t>cell division protein FtsH</t>
+  </si>
+  <si>
+    <t>transposase is3 is911 family protein</t>
+  </si>
+  <si>
+    <t>transposition protein, TnsD-like protein</t>
+  </si>
+  <si>
+    <t>tnsC</t>
+  </si>
+  <si>
+    <t>transporter, AcrB/AcrD/AcrF family</t>
+  </si>
+  <si>
+    <t>PA5409 (PI: 38.6%)</t>
+  </si>
+  <si>
+    <t>PA3126 (PI: 35.8%)</t>
+  </si>
+  <si>
+    <t>heat-shock protein IbpA</t>
+  </si>
+  <si>
+    <t>PA4751 (PI: 45.7%)</t>
+  </si>
+  <si>
+    <t>PA0983 (PI: 29.5%)</t>
+  </si>
+  <si>
+    <t>conserved hypothetical protein</t>
   </si>
 </sst>
 </file>
@@ -454,41 +547,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -514,18 +610,18 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>-2.1056525055348154</v>
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -537,53 +633,53 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.3665600236878064</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.7388028817618921</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.4210031910968908</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.4788703088691024</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.3204184159995824</v>
+        <v>-2.1056525055348154</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -591,28 +687,28 @@
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>2.2153384304049895</v>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.6138993995334041</v>
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -624,27 +720,27 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>3.3590769054450647</v>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -653,27 +749,27 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1.5572870179685228</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.7127047041210373</v>
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -682,103 +778,451 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.8477759475142188</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.1402104509060926</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.3386654707028187</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3.8777444476514771</v>
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.3665600236878064</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7388028817618921</v>
       </c>
       <c r="D10" s="1">
-        <v>1.3849237230073144</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>1.4210031910968908</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.4788703088691024</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.3204184159995824</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.2153384304049895</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.6138993995334041</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.3590769054450647</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.5572870179685228</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.7127047041210373</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.8477759475142188</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.1402104509060926</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.3386654707028187</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3.8777444476514771</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.3849237230073144</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.432502109928822</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.6583655189506026</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1.432502109928822</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1.6583655189506026</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>31</v>
+      <c r="H23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of ComplexHeatmap Analysis file for small prescreened datasets, along with the creation of a function for producing both numbered and plane Heatmaps with the function (need to create second function)
</commit_message>
<xml_diff>
--- a/Analysis Temp X vs X/Secondary Analyses/CF39 25_vs_OtherTemps/TnT CF39 thermoregulation Shrunk2.xlsx
+++ b/Analysis Temp X vs X/Secondary Analyses/CF39 25_vs_OtherTemps/TnT CF39 thermoregulation Shrunk2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="69">
   <si>
     <t>PROKKA_06325_sense</t>
   </si>
@@ -110,12 +110,6 @@
     <t>product</t>
   </si>
   <si>
-    <t>PAO1 ID (Pseudomonas DB Protein search)</t>
-  </si>
-  <si>
-    <t>Protein Description</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -219,6 +213,24 @@
   </si>
   <si>
     <t>conserved hypothetical protein</t>
+  </si>
+  <si>
+    <t>Protein Description (Pseudomonas DB Protein search)</t>
+  </si>
+  <si>
+    <t>PAO1 ID Nucleotide (Pseudomonas DB Nucleotide search)</t>
+  </si>
+  <si>
+    <t>Nucleotide Description (Pseudomonas DB Nucleotide search)</t>
+  </si>
+  <si>
+    <t>PAO1 ID Protein (Pseudomonas DB Protein search)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA0459 (PI: 77.5%, PC: 69.1%) </t>
+  </si>
+  <si>
+    <t>probable ClpA/B Protease</t>
   </si>
 </sst>
 </file>
@@ -547,18 +559,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K19" sqref="K19:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -581,13 +598,19 @@
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,44 +633,56 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -665,16 +700,22 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -691,79 +732,97 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -784,15 +843,21 @@
         <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -813,13 +878,19 @@
         <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -842,13 +913,19 @@
         <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -871,15 +948,21 @@
         <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -900,44 +983,56 @@
         <v>13</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -958,13 +1053,19 @@
         <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -987,13 +1088,19 @@
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1016,13 +1123,19 @@
         <v>13</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1045,13 +1158,19 @@
         <v>13</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1074,15 +1193,21 @@
         <v>16</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -1100,16 +1225,22 @@
         <v>6</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1132,15 +1263,21 @@
         <v>18</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -1158,45 +1295,57 @@
         <v>6</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1219,10 +1368,16 @@
         <v>20</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>